<commit_message>
Minor adjustments; Added a country-specific parameter SAVINGS_RATE to be loaded from the parameters.xlsx input file.
</commit_message>
<xml_diff>
--- a/input/EL/columns_number_parameters.xlsx
+++ b/input/EL/columns_number_parameters.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEU/input/EL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1382586D-A1CE-D946-B9B1-8733F3EF78B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A75E094-0C76-924D-B087-711FBED17EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="22760" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="22760" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnsNumberParameters" sheetId="1" r:id="rId1"/>
+    <sheet name="Info" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>KEY</t>
   </si>
@@ -131,13 +132,84 @@
   </si>
   <si>
     <t>columnsRetirementR1b</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This Excel file is used to define the column numbers required for the corresponding processes in the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>reg_estimates</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> files.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Since the column numbers differ by country, they must be configured </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>separately</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>each country</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +222,21 @@
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -172,17 +259,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,7 +575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -508,26 +594,26 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -783,4 +869,32 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41713FEA-DEF4-7447-A8C4-624BC2867DFC}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="92.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adjusted and unified the necessary parameters. Additionally, introduced new parameters for the hard-coded values.
</commit_message>
<xml_diff>
--- a/input/EL/columns_number_parameters.xlsx
+++ b/input/EL/columns_number_parameters.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEU/input/EL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A75E094-0C76-924D-B087-711FBED17EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E815D2-DE05-4A4E-A4C4-70C7F25AB70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="22760" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="22760" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ColumnsNumberParameters" sheetId="1" r:id="rId1"/>
+    <sheet name="ColumnsNumberParameters" sheetId="3" r:id="rId1"/>
     <sheet name="Info" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>KEY</t>
   </si>
@@ -203,6 +203,33 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>columnsProjectionsHighEdu</t>
+  </si>
+  <si>
+    <t>columnsProjectionsLowEdu</t>
+  </si>
+  <si>
+    <t>columnsStudentShareProjections</t>
+  </si>
+  <si>
+    <t>columnsEmploymentAlignment</t>
+  </si>
+  <si>
+    <t>columnsFertilityProjectionsByYear</t>
+  </si>
+  <si>
+    <t>columnsCoefficientMapRMSE</t>
+  </si>
+  <si>
+    <t>columnsMortalityProbabilityByGenderAgeYear</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>columnsPopulationProjections</t>
   </si>
 </sst>
 </file>
@@ -259,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -269,6 +296,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,18 +600,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DA6936-DB5C-1446-A0B0-CD16C8DB82E1}">
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="42.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -865,9 +889,72 @@
         <v>27</v>
       </c>
     </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -875,7 +962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41713FEA-DEF4-7447-A8C4-624BC2867DFC}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
The model has been updated to support a country-specific approach for managing F1a.
</commit_message>
<xml_diff>
--- a/input/EL/columns_number_parameters.xlsx
+++ b/input/EL/columns_number_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEU/input/EL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E815D2-DE05-4A4E-A4C4-70C7F25AB70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197AE2ED-F25C-B047-AF1C-E29DDE7EFCE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="22760" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18520" yWindow="1540" windowWidth="22760" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnsNumberParameters" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>KEY</t>
   </si>
@@ -230,6 +230,12 @@
   </si>
   <si>
     <t>columnsPopulationProjections</t>
+  </si>
+  <si>
+    <t>columnsFertilityF1a</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -601,13 +607,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DA6936-DB5C-1446-A0B0-CD16C8DB82E1}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -819,87 +828,87 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="1">
-        <v>28</v>
+        <v>48</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="1">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1">
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B36" s="1">
         <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36">
-        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -907,15 +916,15 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39">
         <v>40</v>
@@ -923,33 +932,41 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40">
-        <v>90</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B42">
-        <v>111</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B44" s="5" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Person.java and columns_number*.xlsx for EL Update was needed to account for updated estimation of the leaveParentalHome process (P1a)
</commit_message>
<xml_diff>
--- a/input/EL/columns_number_parameters.xlsx
+++ b/input/EL/columns_number_parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEU/input/EL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEUmerged/input/EL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197AE2ED-F25C-B047-AF1C-E29DDE7EFCE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5299FF4A-21E5-BF4F-8D43-7A9F96F7747D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18520" yWindow="1540" windowWidth="22760" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>KEY</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>26</t>
   </si>
 </sst>
 </file>
@@ -292,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -303,6 +306,7 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -878,8 +882,8 @@
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="1">
-        <v>17</v>
+      <c r="B33" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated Partnership - removed previsouly_partnered category and renamed "SingleNeverMarried" into "Single" - updated fertility estimates for all 4 countries (that also required updating columns_numbers_parameters.xlsx) - Greece (EL) does not have estimates for F1a - so I adjusted the code accordingly using FLAG_SKIP_F1A
</commit_message>
<xml_diff>
--- a/input/EL/columns_number_parameters.xlsx
+++ b/input/EL/columns_number_parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEUmerged/input/EL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEU_NOV/input/EL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5299FF4A-21E5-BF4F-8D43-7A9F96F7747D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50435DAE-C348-E549-9872-B89C76847674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18520" yWindow="1540" windowWidth="22760" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>KEY</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>26</t>
+  </si>
+  <si>
+    <t>34</t>
   </si>
 </sst>
 </file>
@@ -295,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -307,6 +310,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,7 +618,7 @@
   <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -842,8 +846,8 @@
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="1">
-        <v>28</v>
+      <c r="B28" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>